<commit_message>
Add 2nd test + data from excel
</commit_message>
<xml_diff>
--- a/src/test/resources/exel/testdata.xlsx
+++ b/src/test/resources/exel/testdata.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/repos/DataDriven/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/repos/DataDriven/src/test/resources/exel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4CB3745-6FD2-7E44-8AE5-809C07D7748F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BCBB93-A7B3-1C4E-A945-375907222A51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16200" xr2:uid="{2320DFE5-DEA2-1D45-9ADB-0A9634BE0859}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,6 +22,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>Katya</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>ab214c</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,12 +395,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C48A59FF-BABA-9A4E-8CB7-69C4CB81143D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add listeners and reports
</commit_message>
<xml_diff>
--- a/src/test/resources/exel/testdata.xlsx
+++ b/src/test/resources/exel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/repos/DataDriven/src/test/resources/exel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BCBB93-A7B3-1C4E-A945-375907222A51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3506844-BE85-664A-9FC1-16BB916A573B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16200" xr2:uid="{2320DFE5-DEA2-1D45-9ADB-0A9634BE0859}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>firstname</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>ab214c</t>
+  </si>
+  <si>
+    <t>alerttext</t>
+  </si>
+  <si>
+    <t>Customer added successfully</t>
   </si>
 </sst>
 </file>
@@ -395,15 +401,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C48A59FF-BABA-9A4E-8CB7-69C4CB81143D}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,8 +422,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -423,6 +435,9 @@
       </c>
       <c r="C2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD dataProviderClass and new test case OpenAccountTest
</commit_message>
<xml_diff>
--- a/src/test/resources/exel/testdata.xlsx
+++ b/src/test/resources/exel/testdata.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/repos/DataDriven/src/test/resources/exel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3506844-BE85-664A-9FC1-16BB916A573B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DC0FC2-B2B9-C947-B225-47BD0B377585}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16200" xr2:uid="{2320DFE5-DEA2-1D45-9ADB-0A9634BE0859}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16200" activeTab="1" xr2:uid="{2320DFE5-DEA2-1D45-9ADB-0A9634BE0859}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>firstname</t>
   </si>
@@ -49,6 +50,18 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Katya Smith</t>
+  </si>
+  <si>
+    <t>Dollar</t>
   </si>
 </sst>
 </file>
@@ -403,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C48A59FF-BABA-9A4E-8CB7-69C4CB81143D}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -443,4 +456,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA151D6-B2FD-914F-935D-8FF8F224E92A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>